<commit_message>
changed id variable to d_id
added in column f impossible in all respective lines
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S3_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S3_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A6541E-634C-4981-ABF9-E604BBEB0679}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{0DC89B52-5B10-4A06-9106-C32747F8F37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="444">
   <si>
     <t>index</t>
   </si>
@@ -1482,9 +1482,6 @@
     <t>intake of amphibians, reptiles, snails, insects [g/d]</t>
   </si>
   <si>
-    <t>D_ID</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -1499,6 +1496,9 @@
 DV147 (bacon) + 
 DV150 (canned, frozen meat or meat products) + 
 DV160 (other meat products)</t>
+  </si>
+  <si>
+    <t>d_id</t>
   </si>
 </sst>
 </file>
@@ -2097,9 +2097,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2120,6 +2117,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2479,27 +2479,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="7"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="7"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="8"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2534,14 +2534,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="C2" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -2550,8 +2550,8 @@
       <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>439</v>
+      <c r="F2" s="32" t="s">
+        <v>443</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>13</v>
@@ -2569,14 +2569,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2602,14 +2602,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -2635,14 +2635,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -2668,14 +2668,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -2701,14 +2701,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -2734,7 +2734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -2750,7 +2750,7 @@
       <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>37</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -2767,7 +2767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -2783,7 +2783,7 @@
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -2800,14 +2800,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -2835,14 +2835,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -2851,7 +2851,7 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -2870,14 +2870,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -2886,7 +2886,9 @@
       <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>56</v>
       </c>
@@ -2901,14 +2903,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -2917,7 +2919,7 @@
       <c r="E13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="34" t="s">
         <v>59</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2936,14 +2938,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -2971,14 +2973,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -3006,14 +3008,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -3041,14 +3043,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>77</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -3076,14 +3078,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="31" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -3092,7 +3094,9 @@
       <c r="E18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>56</v>
       </c>
@@ -3106,14 +3110,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>84</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -3122,7 +3126,9 @@
       <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>56</v>
       </c>
@@ -3137,14 +3143,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>86</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -3172,14 +3178,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="31" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -3207,14 +3213,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>92</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -3223,7 +3229,9 @@
       <c r="E22" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>56</v>
       </c>
@@ -3238,14 +3246,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="31" t="s">
         <v>94</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -3273,14 +3281,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="31" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -3289,7 +3297,9 @@
       <c r="E24" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G24" s="2" t="s">
         <v>56</v>
       </c>
@@ -3304,14 +3314,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="31" t="s">
         <v>100</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -3339,14 +3349,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="31" t="s">
         <v>105</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -3374,14 +3384,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>110</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -3409,14 +3419,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="31" t="s">
         <v>114</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -3444,14 +3454,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="31" t="s">
         <v>119</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -3460,7 +3470,9 @@
       <c r="E29" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G29" s="2" t="s">
         <v>56</v>
       </c>
@@ -3475,14 +3487,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="31" t="s">
         <v>121</v>
       </c>
       <c r="D30" s="8" t="s">
@@ -3510,14 +3522,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>126</v>
       </c>
       <c r="D31" s="8" t="s">
@@ -3545,14 +3557,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -3561,7 +3573,9 @@
       <c r="E32" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G32" s="2" t="s">
         <v>56</v>
       </c>
@@ -3576,14 +3590,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="31" t="s">
         <v>132</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -3611,14 +3625,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="31" t="s">
         <v>136</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3646,14 +3660,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="31" t="s">
         <v>140</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -3681,14 +3695,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="31" t="s">
         <v>144</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -3697,7 +3711,9 @@
       <c r="E36" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G36" s="2" t="s">
         <v>56</v>
       </c>
@@ -3711,14 +3727,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="31" t="s">
         <v>146</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -3727,7 +3743,9 @@
       <c r="E37" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G37" s="2" t="s">
         <v>56</v>
       </c>
@@ -3742,14 +3760,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="31" t="s">
         <v>148</v>
       </c>
       <c r="D38" s="8" t="s">
@@ -3777,14 +3795,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="31" t="s">
         <v>152</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -3793,7 +3811,9 @@
       <c r="E39" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G39" s="2" t="s">
         <v>56</v>
       </c>
@@ -3808,14 +3828,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>154</v>
       </c>
       <c r="D40" s="8" t="s">
@@ -3843,14 +3863,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="31" t="s">
         <v>158</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -3878,14 +3898,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="31" t="s">
         <v>163</v>
       </c>
       <c r="D42" s="8" t="s">
@@ -3913,14 +3933,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="31" t="s">
         <v>168</v>
       </c>
       <c r="D43" s="8" t="s">
@@ -3948,14 +3968,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>173</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -3984,14 +4004,14 @@
       </c>
       <c r="L44" s="11"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="31" t="s">
         <v>178</v>
       </c>
       <c r="D45" s="8" t="s">
@@ -4019,14 +4039,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="31" t="s">
         <v>183</v>
       </c>
       <c r="D46" s="8" t="s">
@@ -4054,14 +4074,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="31" t="s">
         <v>187</v>
       </c>
       <c r="D47" s="8" t="s">
@@ -4070,7 +4090,9 @@
       <c r="E47" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G47" s="2" t="s">
         <v>56</v>
       </c>
@@ -4084,14 +4106,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="31" t="s">
         <v>189</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -4100,7 +4122,9 @@
       <c r="E48" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G48" s="2" t="s">
         <v>56</v>
       </c>
@@ -4114,14 +4138,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="31" t="s">
         <v>191</v>
       </c>
       <c r="D49" s="8" t="s">
@@ -4130,7 +4154,9 @@
       <c r="E49" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G49" s="2" t="s">
         <v>30</v>
       </c>
@@ -4147,14 +4173,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="31" t="s">
         <v>194</v>
       </c>
       <c r="D50" s="8" t="s">
@@ -4182,14 +4208,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="31" t="s">
         <v>199</v>
       </c>
       <c r="D51" s="8" t="s">
@@ -4217,14 +4243,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C52" s="31" t="s">
         <v>204</v>
       </c>
       <c r="D52" s="8" t="s">
@@ -4252,14 +4278,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="31" t="s">
         <v>208</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -4287,14 +4313,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C54" s="31" t="s">
         <v>212</v>
       </c>
       <c r="D54" s="8" t="s">
@@ -4322,14 +4348,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C55" s="32" t="s">
+      <c r="C55" s="31" t="s">
         <v>216</v>
       </c>
       <c r="D55" s="8" t="s">
@@ -4347,7 +4373,7 @@
       <c r="H55" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="I55" s="28" t="s">
+      <c r="I55" s="27" t="s">
         <v>219</v>
       </c>
       <c r="J55" s="1" t="s">
@@ -4357,14 +4383,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="31" t="s">
         <v>221</v>
       </c>
       <c r="D56" s="8" t="s">
@@ -4373,7 +4399,9 @@
       <c r="E56" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G56" s="2" t="s">
         <v>56</v>
       </c>
@@ -4388,14 +4416,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C57" s="32" t="s">
+      <c r="C57" s="31" t="s">
         <v>223</v>
       </c>
       <c r="D57" s="8" t="s">
@@ -4413,7 +4441,7 @@
       <c r="H57" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="I57" s="28" t="s">
+      <c r="I57" s="27" t="s">
         <v>219</v>
       </c>
       <c r="J57" s="1" t="s">
@@ -4423,14 +4451,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="31" t="s">
         <v>226</v>
       </c>
       <c r="D58" s="8" t="s">
@@ -4458,14 +4486,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="31" t="s">
         <v>230</v>
       </c>
       <c r="D59" s="8" t="s">
@@ -4474,7 +4502,9 @@
       <c r="E59" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G59" s="2" t="s">
         <v>56</v>
       </c>
@@ -4489,14 +4519,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="31" t="s">
         <v>232</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -4505,7 +4535,9 @@
       <c r="E60" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G60" s="2" t="s">
         <v>56</v>
       </c>
@@ -4520,14 +4552,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="31" t="s">
         <v>234</v>
       </c>
       <c r="D61" s="8" t="s">
@@ -4536,7 +4568,9 @@
       <c r="E61" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G61" s="2" t="s">
         <v>56</v>
       </c>
@@ -4551,14 +4585,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C62" s="32" t="s">
+      <c r="C62" s="31" t="s">
         <v>236</v>
       </c>
       <c r="D62" s="8" t="s">
@@ -4567,7 +4601,9 @@
       <c r="E62" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G62" s="2" t="s">
         <v>56</v>
       </c>
@@ -4582,14 +4618,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="31" t="s">
         <v>238</v>
       </c>
       <c r="D63" s="8" t="s">
@@ -4598,7 +4634,9 @@
       <c r="E63" t="s">
         <v>12</v>
       </c>
-      <c r="F63" s="2"/>
+      <c r="F63" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G63" s="2" t="s">
         <v>56</v>
       </c>
@@ -4613,14 +4651,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="31" t="s">
         <v>240</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -4629,7 +4667,9 @@
       <c r="E64" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G64" s="2" t="s">
         <v>56</v>
       </c>
@@ -4644,14 +4684,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="31" t="s">
         <v>242</v>
       </c>
       <c r="D65" s="8" t="s">
@@ -4679,14 +4719,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="31" t="s">
         <v>246</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -4696,16 +4736,16 @@
         <v>12</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H66" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I66" s="33" t="s">
         <v>442</v>
-      </c>
-      <c r="I66" s="34" t="s">
-        <v>443</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>52</v>
@@ -4714,14 +4754,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="31" t="s">
         <v>248</v>
       </c>
       <c r="D67" s="8" t="s">
@@ -4749,14 +4789,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="31" t="s">
         <v>252</v>
       </c>
       <c r="D68" s="8" t="s">
@@ -4784,14 +4824,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C69" s="32" t="s">
+      <c r="C69" s="31" t="s">
         <v>257</v>
       </c>
       <c r="D69" s="8" t="s">
@@ -4819,14 +4859,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C70" s="32" t="s">
+      <c r="C70" s="31" t="s">
         <v>261</v>
       </c>
       <c r="D70" s="8" t="s">
@@ -4835,7 +4875,9 @@
       <c r="E70" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="2"/>
+      <c r="F70" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G70" s="2" t="s">
         <v>56</v>
       </c>
@@ -4850,14 +4892,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C71" s="32" t="s">
+      <c r="C71" s="31" t="s">
         <v>263</v>
       </c>
       <c r="D71" s="8" t="s">
@@ -4885,14 +4927,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>267</v>
       </c>
-      <c r="C72" s="32" t="s">
+      <c r="C72" s="31" t="s">
         <v>268</v>
       </c>
       <c r="D72" s="8" t="s">
@@ -4920,14 +4962,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>272</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="31" t="s">
         <v>273</v>
       </c>
       <c r="D73" s="8" t="s">
@@ -4955,14 +4997,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>276</v>
       </c>
-      <c r="C74" s="32" t="s">
+      <c r="C74" s="31" t="s">
         <v>277</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -4990,14 +5032,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>281</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C75" s="31" t="s">
         <v>282</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -5025,14 +5067,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>285</v>
       </c>
-      <c r="C76" s="32" t="s">
+      <c r="C76" s="31" t="s">
         <v>286</v>
       </c>
       <c r="D76" s="8" t="s">
@@ -5060,14 +5102,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>289</v>
       </c>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="31" t="s">
         <v>290</v>
       </c>
       <c r="D77" s="8" t="s">
@@ -5095,14 +5137,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>293</v>
       </c>
-      <c r="C78" s="32" t="s">
+      <c r="C78" s="31" t="s">
         <v>294</v>
       </c>
       <c r="D78" s="8" t="s">
@@ -5111,7 +5153,9 @@
       <c r="E78" t="s">
         <v>12</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G78" s="2" t="s">
         <v>56</v>
       </c>
@@ -5126,14 +5170,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>295</v>
       </c>
-      <c r="C79" s="32" t="s">
+      <c r="C79" s="31" t="s">
         <v>296</v>
       </c>
       <c r="D79" s="8" t="s">
@@ -5142,7 +5186,9 @@
       <c r="E79" t="s">
         <v>12</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G79" s="2" t="s">
         <v>56</v>
       </c>
@@ -5156,14 +5202,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>297</v>
       </c>
-      <c r="C80" s="32" t="s">
+      <c r="C80" s="31" t="s">
         <v>298</v>
       </c>
       <c r="D80" s="8" t="s">
@@ -5172,7 +5218,9 @@
       <c r="E80" t="s">
         <v>12</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G80" s="2" t="s">
         <v>56</v>
       </c>
@@ -5186,14 +5234,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>299</v>
       </c>
-      <c r="C81" s="32" t="s">
+      <c r="C81" s="31" t="s">
         <v>300</v>
       </c>
       <c r="D81" s="8" t="s">
@@ -5221,14 +5269,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>304</v>
       </c>
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="31" t="s">
         <v>305</v>
       </c>
       <c r="D82" s="8" t="s">
@@ -5256,14 +5304,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>309</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="C83" s="31" t="s">
         <v>310</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -5291,14 +5339,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>314</v>
       </c>
-      <c r="C84" s="32" t="s">
+      <c r="C84" s="31" t="s">
         <v>315</v>
       </c>
       <c r="D84" s="8" t="s">
@@ -5326,14 +5374,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>318</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="C85" s="31" t="s">
         <v>319</v>
       </c>
       <c r="D85" s="8" t="s">
@@ -5342,7 +5390,9 @@
       <c r="E85" t="s">
         <v>12</v>
       </c>
-      <c r="F85" s="2"/>
+      <c r="F85" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G85" s="2" t="s">
         <v>56</v>
       </c>
@@ -5357,14 +5407,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>320</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="C86" s="31" t="s">
         <v>321</v>
       </c>
       <c r="D86" s="8" t="s">
@@ -5373,7 +5423,9 @@
       <c r="E86" t="s">
         <v>12</v>
       </c>
-      <c r="F86" s="2"/>
+      <c r="F86" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G86" s="2" t="s">
         <v>56</v>
       </c>
@@ -5387,14 +5439,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>322</v>
       </c>
-      <c r="C87" s="32" t="s">
+      <c r="C87" s="31" t="s">
         <v>323</v>
       </c>
       <c r="D87" s="8" t="s">
@@ -5422,14 +5474,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>326</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="C88" s="31" t="s">
         <v>327</v>
       </c>
       <c r="D88" s="8" t="s">
@@ -5438,7 +5490,9 @@
       <c r="E88" t="s">
         <v>12</v>
       </c>
-      <c r="F88" s="2"/>
+      <c r="F88" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G88" s="2" t="s">
         <v>56</v>
       </c>
@@ -5453,14 +5507,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>328</v>
       </c>
-      <c r="C89" s="32" t="s">
+      <c r="C89" s="31" t="s">
         <v>329</v>
       </c>
       <c r="D89" s="8" t="s">
@@ -5469,7 +5523,9 @@
       <c r="E89" t="s">
         <v>12</v>
       </c>
-      <c r="F89" s="2"/>
+      <c r="F89" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G89" s="2" t="s">
         <v>56</v>
       </c>
@@ -5484,14 +5540,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>330</v>
       </c>
-      <c r="C90" s="32" t="s">
+      <c r="C90" s="31" t="s">
         <v>331</v>
       </c>
       <c r="D90" s="8" t="s">
@@ -5519,14 +5575,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>335</v>
       </c>
-      <c r="C91" s="32" t="s">
+      <c r="C91" s="31" t="s">
         <v>336</v>
       </c>
       <c r="D91" s="8" t="s">
@@ -5535,7 +5591,9 @@
       <c r="E91" t="s">
         <v>12</v>
       </c>
-      <c r="F91" s="2"/>
+      <c r="F91" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G91" s="2" t="s">
         <v>56</v>
       </c>
@@ -5550,14 +5608,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>337</v>
       </c>
-      <c r="C92" s="32" t="s">
+      <c r="C92" s="31" t="s">
         <v>338</v>
       </c>
       <c r="D92" s="8" t="s">
@@ -5566,7 +5624,9 @@
       <c r="E92" t="s">
         <v>12</v>
       </c>
-      <c r="F92" s="2"/>
+      <c r="F92" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G92" s="2" t="s">
         <v>56</v>
       </c>
@@ -5581,14 +5641,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>339</v>
       </c>
-      <c r="C93" s="32" t="s">
+      <c r="C93" s="31" t="s">
         <v>340</v>
       </c>
       <c r="D93" s="8" t="s">
@@ -5616,14 +5676,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>344</v>
       </c>
-      <c r="C94" s="32" t="s">
+      <c r="C94" s="31" t="s">
         <v>345</v>
       </c>
       <c r="D94" s="8" t="s">
@@ -5651,14 +5711,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>348</v>
       </c>
-      <c r="C95" s="32" t="s">
+      <c r="C95" s="31" t="s">
         <v>349</v>
       </c>
       <c r="D95" s="8" t="s">
@@ -5686,14 +5746,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>353</v>
       </c>
-      <c r="C96" s="32" t="s">
+      <c r="C96" s="31" t="s">
         <v>354</v>
       </c>
       <c r="D96" s="8" t="s">
@@ -5721,14 +5781,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>358</v>
       </c>
-      <c r="C97" s="32" t="s">
+      <c r="C97" s="31" t="s">
         <v>359</v>
       </c>
       <c r="D97" s="8" t="s">
@@ -5756,14 +5816,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>363</v>
       </c>
-      <c r="C98" s="32" t="s">
+      <c r="C98" s="31" t="s">
         <v>364</v>
       </c>
       <c r="D98" s="8" t="s">
@@ -5791,14 +5851,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>367</v>
       </c>
-      <c r="C99" s="32" t="s">
+      <c r="C99" s="31" t="s">
         <v>368</v>
       </c>
       <c r="D99" s="8" t="s">
@@ -5807,7 +5867,9 @@
       <c r="E99" t="s">
         <v>12</v>
       </c>
-      <c r="F99" s="2"/>
+      <c r="F99" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G99" s="2" t="s">
         <v>56</v>
       </c>
@@ -5821,14 +5883,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>369</v>
       </c>
-      <c r="C100" s="32" t="s">
+      <c r="C100" s="31" t="s">
         <v>370</v>
       </c>
       <c r="D100" s="8" t="s">
@@ -5837,7 +5899,9 @@
       <c r="E100" t="s">
         <v>12</v>
       </c>
-      <c r="F100" s="2"/>
+      <c r="F100" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G100" s="2" t="s">
         <v>56</v>
       </c>
@@ -5852,14 +5916,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>371</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="C101" s="31" t="s">
         <v>372</v>
       </c>
       <c r="D101" s="8" t="s">
@@ -5887,14 +5951,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>375</v>
       </c>
-      <c r="C102" s="32" t="s">
+      <c r="C102" s="31" t="s">
         <v>376</v>
       </c>
       <c r="D102" s="8" t="s">
@@ -5922,14 +5986,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>380</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="C103" s="31" t="s">
         <v>381</v>
       </c>
       <c r="D103" s="8" t="s">
@@ -5957,14 +6021,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>385</v>
       </c>
-      <c r="C104" s="32" t="s">
+      <c r="C104" s="31" t="s">
         <v>386</v>
       </c>
       <c r="D104" s="8" t="s">
@@ -5973,7 +6037,9 @@
       <c r="E104" t="s">
         <v>12</v>
       </c>
-      <c r="F104" s="2"/>
+      <c r="F104" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G104" s="2" t="s">
         <v>56</v>
       </c>
@@ -5988,14 +6054,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>387</v>
       </c>
-      <c r="C105" s="32" t="s">
+      <c r="C105" s="31" t="s">
         <v>388</v>
       </c>
       <c r="D105" s="8" t="s">
@@ -6023,14 +6089,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>391</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="C106" s="31" t="s">
         <v>392</v>
       </c>
       <c r="D106" s="8" t="s">
@@ -6058,14 +6124,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>395</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="C107" s="31" t="s">
         <v>396</v>
       </c>
       <c r="D107" s="8" t="s">
@@ -6074,7 +6140,9 @@
       <c r="E107" t="s">
         <v>12</v>
       </c>
-      <c r="F107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G107" s="2" t="s">
         <v>56</v>
       </c>
@@ -6088,14 +6156,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>397</v>
       </c>
-      <c r="C108" s="32" t="s">
+      <c r="C108" s="31" t="s">
         <v>398</v>
       </c>
       <c r="D108" s="8" t="s">
@@ -6104,7 +6172,9 @@
       <c r="E108" t="s">
         <v>12</v>
       </c>
-      <c r="F108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G108" s="2" t="s">
         <v>56</v>
       </c>
@@ -6118,14 +6188,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>399</v>
       </c>
-      <c r="C109" s="32" t="s">
+      <c r="C109" s="31" t="s">
         <v>400</v>
       </c>
       <c r="D109" s="8" t="s">
@@ -6134,7 +6204,9 @@
       <c r="E109" t="s">
         <v>12</v>
       </c>
-      <c r="F109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G109" s="2" t="s">
         <v>56</v>
       </c>
@@ -6148,14 +6220,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>401</v>
       </c>
-      <c r="C110" s="32" t="s">
+      <c r="C110" s="31" t="s">
         <v>402</v>
       </c>
       <c r="D110" s="8" t="s">
@@ -6164,7 +6236,9 @@
       <c r="E110" t="s">
         <v>12</v>
       </c>
-      <c r="F110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G110" s="2" t="s">
         <v>56</v>
       </c>
@@ -6178,14 +6252,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>403</v>
       </c>
-      <c r="C111" s="32" t="s">
+      <c r="C111" s="31" t="s">
         <v>404</v>
       </c>
       <c r="D111" s="8" t="s">
@@ -6194,7 +6268,9 @@
       <c r="E111" t="s">
         <v>12</v>
       </c>
-      <c r="F111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G111" s="2" t="s">
         <v>56</v>
       </c>
@@ -6209,14 +6285,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>111</v>
       </c>
       <c r="B112" t="s">
         <v>405</v>
       </c>
-      <c r="C112" s="32" t="s">
+      <c r="C112" s="31" t="s">
         <v>406</v>
       </c>
       <c r="D112" s="8" t="s">
@@ -6225,7 +6301,9 @@
       <c r="E112" t="s">
         <v>12</v>
       </c>
-      <c r="F112" s="2"/>
+      <c r="F112" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G112" s="2" t="s">
         <v>56</v>
       </c>
@@ -6240,14 +6318,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>407</v>
       </c>
-      <c r="C113" s="32" t="s">
+      <c r="C113" s="31" t="s">
         <v>408</v>
       </c>
       <c r="D113" s="8" t="s">
@@ -6256,7 +6334,9 @@
       <c r="E113" t="s">
         <v>12</v>
       </c>
-      <c r="F113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G113" s="2" t="s">
         <v>56</v>
       </c>
@@ -6271,14 +6351,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
         <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>409</v>
       </c>
-      <c r="C114" s="32" t="s">
+      <c r="C114" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D114" s="8" t="s">
@@ -6287,7 +6367,9 @@
       <c r="E114" t="s">
         <v>12</v>
       </c>
-      <c r="F114" s="2"/>
+      <c r="F114" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G114" s="2" t="s">
         <v>56</v>
       </c>
@@ -6302,14 +6384,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>411</v>
       </c>
-      <c r="C115" s="32" t="s">
+      <c r="C115" s="31" t="s">
         <v>412</v>
       </c>
       <c r="D115" s="8" t="s">
@@ -6318,7 +6400,9 @@
       <c r="E115" t="s">
         <v>12</v>
       </c>
-      <c r="F115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G115" s="2" t="s">
         <v>56</v>
       </c>
@@ -6333,14 +6417,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>413</v>
       </c>
-      <c r="C116" s="32" t="s">
+      <c r="C116" s="31" t="s">
         <v>414</v>
       </c>
       <c r="D116" s="8" t="s">
@@ -6349,7 +6433,9 @@
       <c r="E116" t="s">
         <v>12</v>
       </c>
-      <c r="F116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G116" s="2" t="s">
         <v>56</v>
       </c>
@@ -6364,14 +6450,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>415</v>
       </c>
-      <c r="C117" s="32" t="s">
+      <c r="C117" s="31" t="s">
         <v>416</v>
       </c>
       <c r="D117" s="8" t="s">
@@ -6380,7 +6466,9 @@
       <c r="E117" t="s">
         <v>12</v>
       </c>
-      <c r="F117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G117" s="2" t="s">
         <v>56</v>
       </c>
@@ -6395,14 +6483,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>417</v>
       </c>
-      <c r="C118" s="32" t="s">
+      <c r="C118" s="31" t="s">
         <v>418</v>
       </c>
       <c r="D118" s="8" t="s">
@@ -6411,7 +6499,9 @@
       <c r="E118" t="s">
         <v>12</v>
       </c>
-      <c r="F118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G118" s="2" t="s">
         <v>56</v>
       </c>
@@ -6426,14 +6516,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>419</v>
       </c>
-      <c r="C119" s="32" t="s">
+      <c r="C119" s="31" t="s">
         <v>420</v>
       </c>
       <c r="D119" s="8" t="s">
@@ -6442,7 +6532,9 @@
       <c r="E119" t="s">
         <v>12</v>
       </c>
-      <c r="F119" s="2"/>
+      <c r="F119" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G119" s="2" t="s">
         <v>56</v>
       </c>
@@ -6456,14 +6548,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>119</v>
       </c>
       <c r="B120" t="s">
         <v>421</v>
       </c>
-      <c r="C120" s="32" t="s">
+      <c r="C120" s="31" t="s">
         <v>422</v>
       </c>
       <c r="D120" s="8" t="s">
@@ -6472,7 +6564,9 @@
       <c r="E120" t="s">
         <v>12</v>
       </c>
-      <c r="F120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G120" s="2" t="s">
         <v>56</v>
       </c>
@@ -6486,14 +6580,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>120</v>
       </c>
       <c r="B121" t="s">
         <v>423</v>
       </c>
-      <c r="C121" s="32" t="s">
+      <c r="C121" s="31" t="s">
         <v>424</v>
       </c>
       <c r="D121" s="8" t="s">
@@ -6502,7 +6596,9 @@
       <c r="E121" t="s">
         <v>12</v>
       </c>
-      <c r="F121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G121" s="2" t="s">
         <v>56</v>
       </c>
@@ -6516,14 +6612,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>425</v>
       </c>
-      <c r="C122" s="32" t="s">
+      <c r="C122" s="31" t="s">
         <v>426</v>
       </c>
       <c r="D122" s="8" t="s">
@@ -6532,7 +6628,9 @@
       <c r="E122" t="s">
         <v>12</v>
       </c>
-      <c r="F122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G122" s="2" t="s">
         <v>56</v>
       </c>
@@ -6546,14 +6644,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>122</v>
       </c>
       <c r="B123" t="s">
         <v>427</v>
       </c>
-      <c r="C123" s="32" t="s">
+      <c r="C123" s="31" t="s">
         <v>428</v>
       </c>
       <c r="D123" s="8" t="s">
@@ -6562,7 +6660,9 @@
       <c r="E123" t="s">
         <v>12</v>
       </c>
-      <c r="F123" s="2"/>
+      <c r="F123" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G123" s="2" t="s">
         <v>56</v>
       </c>
@@ -6576,14 +6676,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="8">
         <v>123</v>
       </c>
       <c r="B124" t="s">
         <v>429</v>
       </c>
-      <c r="C124" s="32" t="s">
+      <c r="C124" s="31" t="s">
         <v>430</v>
       </c>
       <c r="D124" s="8" t="s">
@@ -6592,7 +6692,9 @@
       <c r="E124" t="s">
         <v>12</v>
       </c>
-      <c r="F124" s="2"/>
+      <c r="F124" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G124" s="2" t="s">
         <v>56</v>
       </c>
@@ -6606,14 +6708,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>124</v>
       </c>
       <c r="B125" t="s">
         <v>431</v>
       </c>
-      <c r="C125" s="32" t="s">
+      <c r="C125" s="31" t="s">
         <v>432</v>
       </c>
       <c r="D125" s="8" t="s">
@@ -6622,7 +6724,9 @@
       <c r="E125" t="s">
         <v>12</v>
       </c>
-      <c r="F125" s="2"/>
+      <c r="F125" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G125" s="2" t="s">
         <v>56</v>
       </c>
@@ -6636,14 +6740,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="8">
         <v>125</v>
       </c>
       <c r="B126" t="s">
         <v>433</v>
       </c>
-      <c r="C126" s="32" t="s">
+      <c r="C126" s="31" t="s">
         <v>434</v>
       </c>
       <c r="D126" s="8" t="s">
@@ -6652,7 +6756,9 @@
       <c r="E126" t="s">
         <v>12</v>
       </c>
-      <c r="F126" s="2"/>
+      <c r="F126" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G126" s="2" t="s">
         <v>56</v>
       </c>
@@ -6666,14 +6772,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>126</v>
       </c>
       <c r="B127" t="s">
         <v>435</v>
       </c>
-      <c r="C127" s="32" t="s">
+      <c r="C127" s="31" t="s">
         <v>436</v>
       </c>
       <c r="D127" s="8" t="s">
@@ -6682,7 +6788,9 @@
       <c r="E127" t="s">
         <v>12</v>
       </c>
-      <c r="F127" s="2"/>
+      <c r="F127" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G127" s="2" t="s">
         <v>56</v>
       </c>
@@ -6696,14 +6804,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="8">
         <v>127</v>
       </c>
       <c r="B128" t="s">
         <v>437</v>
       </c>
-      <c r="C128" s="32" t="s">
+      <c r="C128" s="31" t="s">
         <v>438</v>
       </c>
       <c r="D128" s="8" t="s">
@@ -6712,7 +6820,9 @@
       <c r="E128" t="s">
         <v>12</v>
       </c>
-      <c r="F128" s="2"/>
+      <c r="F128" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G128" s="2" t="s">
         <v>56</v>
       </c>
@@ -6732,6 +6842,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -6972,15 +7091,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6994,6 +7104,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7012,27 +7130,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- for legumes I changed harmonisation potential to compatible and harmonisation rule to operation with respective algortihm - for EGGS_0901 I changed DV255 into DV250
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S3_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S3_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C436F9-6332-4135-BE71-D9A7CFEB2BD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767EDB5F-C707-413D-A7BE-B7A6C42BA971}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="450">
   <si>
     <t>index</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t xml:space="preserve">DV491 </t>
-  </si>
-  <si>
-    <t>DV491 (dry legumes) </t>
   </si>
   <si>
     <t>LEGUMES_0301</t>
@@ -932,12 +929,6 @@
     <t>Intake of eggs [g/d]</t>
   </si>
   <si>
-    <t>DV255</t>
-  </si>
-  <si>
-    <t>DV255 (egg products)</t>
-  </si>
-  <si>
     <t>FAT_10</t>
   </si>
   <si>
@@ -1511,6 +1502,18 @@
   </si>
   <si>
     <t>Intake of amphibians, reptiles, snails, insects [g/d]</t>
+  </si>
+  <si>
+    <t>DV491*2</t>
+  </si>
+  <si>
+    <t>double the amount of DV491 (dry legumes) to be comparable to other studies</t>
+  </si>
+  <si>
+    <t>DV250</t>
+  </si>
+  <si>
+    <t>DV250 (fresh eggs)</t>
   </si>
 </sst>
 </file>
@@ -2500,27 +2503,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C129"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="6"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2555,15 +2558,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -2572,7 +2575,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>12</v>
@@ -2590,7 +2593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2763,7 +2766,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>28</v>
@@ -2788,7 +2791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2891,7 +2894,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -2924,7 +2927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2959,7 +2962,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -3099,7 +3102,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -3267,7 +3270,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -3287,30 +3290,30 @@
         <v>93</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>19</v>
+        <v>446</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>94</v>
+        <v>447</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="30" t="s">
         <v>95</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>96</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>28</v>
@@ -3335,33 +3338,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="D25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>99</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I25" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>101</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>50</v>
@@ -3370,33 +3373,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H26" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="20" t="s">
         <v>105</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>106</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>50</v>
@@ -3405,24 +3408,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="D27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
         <v>108</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>109</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>19</v>
@@ -3431,7 +3434,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>50</v>
@@ -3440,33 +3443,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="D28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>115</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>50</v>
@@ -3475,15 +3478,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>117</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>28</v>
@@ -3508,33 +3511,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="D30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>50</v>
@@ -3543,24 +3546,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="D31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>19</v>
@@ -3569,7 +3572,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>50</v>
@@ -3578,15 +3581,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>127</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>128</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>28</v>
@@ -3611,24 +3614,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="D33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
         <v>130</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>131</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>19</v>
@@ -3637,7 +3640,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>50</v>
@@ -3646,24 +3649,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="D34" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>19</v>
@@ -3672,7 +3675,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>50</v>
@@ -3681,24 +3684,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
         <v>137</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>435</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>138</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>19</v>
@@ -3707,7 +3710,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>50</v>
@@ -3716,15 +3719,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
@@ -3748,15 +3751,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="30" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>142</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
@@ -3781,24 +3784,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="D38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>144</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>145</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>19</v>
@@ -3807,7 +3810,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>50</v>
@@ -3816,15 +3819,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
@@ -3849,24 +3852,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="D40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
         <v>149</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" t="s">
-        <v>150</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>19</v>
@@ -3875,7 +3878,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>50</v>
@@ -3884,33 +3887,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>438</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>155</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>50</v>
@@ -3919,33 +3922,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="D42" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H42" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="I42" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="I42" s="22" t="s">
-        <v>160</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>50</v>
@@ -3954,33 +3957,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="D43" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H43" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I43" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="I43" s="21" t="s">
-        <v>165</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>50</v>
@@ -3989,33 +3992,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="D44" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H44" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I44" s="23" t="s">
         <v>169</v>
-      </c>
-      <c r="I44" s="23" t="s">
-        <v>170</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>50</v>
@@ -4025,33 +4028,33 @@
       </c>
       <c r="L44" s="10"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="D45" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H45" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>50</v>
@@ -4060,24 +4063,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="D46" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>178</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>19</v>
@@ -4086,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>50</v>
@@ -4095,15 +4098,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="30" t="s">
         <v>180</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>181</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
@@ -4127,15 +4130,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="30" t="s">
         <v>182</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>183</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
@@ -4159,15 +4162,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
@@ -4185,7 +4188,7 @@
         <v>29</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>29</v>
@@ -4194,33 +4197,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="D50" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I50" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="I50" s="19" t="s">
-        <v>190</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>50</v>
@@ -4229,33 +4232,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="D51" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
         <v>192</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" t="s">
-        <v>193</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H51" t="s">
+        <v>193</v>
+      </c>
+      <c r="I51" s="22" t="s">
         <v>194</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>195</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>50</v>
@@ -4264,24 +4267,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="D52" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>198</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>19</v>
@@ -4290,7 +4293,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>50</v>
@@ -4299,24 +4302,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="D53" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>202</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>19</v>
@@ -4325,7 +4328,7 @@
         <v>19</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>50</v>
@@ -4334,24 +4337,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C54" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="D54" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>206</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>19</v>
@@ -4360,7 +4363,7 @@
         <v>19</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>50</v>
@@ -4369,33 +4372,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C55" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="D55" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H55" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="I55" s="26" t="s">
         <v>211</v>
-      </c>
-      <c r="I55" s="26" t="s">
-        <v>212</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>45</v>
@@ -4404,15 +4407,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" s="30" t="s">
         <v>213</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>214</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>28</v>
@@ -4437,16 +4440,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C57" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C57" s="30" t="s">
-        <v>216</v>
-      </c>
       <c r="D57" s="7" t="s">
         <v>28</v>
       </c>
@@ -4454,16 +4457,16 @@
         <v>11</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>45</v>
@@ -4472,24 +4475,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C58" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="D58" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
         <v>219</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" t="s">
-        <v>220</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>19</v>
@@ -4498,7 +4501,7 @@
         <v>19</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>50</v>
@@ -4507,15 +4510,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>28</v>
@@ -4540,15 +4543,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>28</v>
@@ -4573,15 +4576,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" s="30" t="s">
         <v>224</v>
-      </c>
-      <c r="C61" s="30" t="s">
-        <v>225</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>28</v>
@@ -4606,15 +4609,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C62" s="30" t="s">
         <v>226</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>227</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>28</v>
@@ -4639,15 +4642,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" s="30" t="s">
         <v>228</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>229</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>28</v>
@@ -4672,15 +4675,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C64" s="30" t="s">
         <v>230</v>
-      </c>
-      <c r="C64" s="30" t="s">
-        <v>231</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>28</v>
@@ -4705,24 +4708,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C65" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="C65" s="30" t="s">
+      <c r="D65" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" t="s">
         <v>233</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" t="s">
-        <v>234</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>19</v>
@@ -4731,7 +4734,7 @@
         <v>19</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>50</v>
@@ -4740,16 +4743,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="C66" s="30" t="s">
-        <v>237</v>
-      </c>
       <c r="D66" s="7" t="s">
         <v>28</v>
       </c>
@@ -4757,16 +4760,16 @@
         <v>11</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I66" s="32" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>50</v>
@@ -4775,24 +4778,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C67" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C67" s="30" t="s">
+      <c r="D67" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="s">
         <v>239</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" t="s">
-        <v>240</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>19</v>
@@ -4801,7 +4804,7 @@
         <v>19</v>
       </c>
       <c r="I67" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>50</v>
@@ -4810,33 +4813,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C68" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="D68" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H68" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="I68" s="19" t="s">
         <v>245</v>
-      </c>
-      <c r="I68" s="19" t="s">
-        <v>246</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>50</v>
@@ -4845,24 +4848,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C69" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
         <v>247</v>
-      </c>
-      <c r="C69" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>248</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>19</v>
@@ -4871,7 +4874,7 @@
         <v>19</v>
       </c>
       <c r="I69" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>50</v>
@@ -4880,15 +4883,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C70" s="30" t="s">
         <v>250</v>
-      </c>
-      <c r="C70" s="30" t="s">
-        <v>251</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>28</v>
@@ -4913,33 +4916,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="C71" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E71" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>253</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H71" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="I71" s="22" t="s">
         <v>254</v>
-      </c>
-      <c r="I71" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>50</v>
@@ -4948,33 +4951,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>255</v>
+      </c>
+      <c r="C72" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="C72" s="30" t="s">
+      <c r="D72" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="15" t="s">
         <v>257</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E72" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>258</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H72" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="I72" s="21" t="s">
         <v>259</v>
-      </c>
-      <c r="I72" s="21" t="s">
-        <v>260</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>50</v>
@@ -4983,16 +4986,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>260</v>
+      </c>
+      <c r="C73" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="C73" s="30" t="s">
-        <v>262</v>
-      </c>
       <c r="D73" s="7" t="s">
         <v>28</v>
       </c>
@@ -5000,7 +5003,7 @@
         <v>11</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>263</v>
+        <v>448</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>19</v>
@@ -5009,7 +5012,7 @@
         <v>19</v>
       </c>
       <c r="I73" s="21" t="s">
-        <v>264</v>
+        <v>449</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>50</v>
@@ -5018,15 +5021,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>28</v>
@@ -5035,16 +5038,16 @@
         <v>11</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>50</v>
@@ -5053,15 +5056,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>28</v>
@@ -5070,7 +5073,7 @@
         <v>11</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>19</v>
@@ -5079,7 +5082,7 @@
         <v>19</v>
       </c>
       <c r="I75" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>50</v>
@@ -5088,15 +5091,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>28</v>
@@ -5105,7 +5108,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>19</v>
@@ -5114,7 +5117,7 @@
         <v>19</v>
       </c>
       <c r="I76" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>50</v>
@@ -5123,15 +5126,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C77" s="30" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>28</v>
@@ -5140,7 +5143,7 @@
         <v>11</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>19</v>
@@ -5149,7 +5152,7 @@
         <v>19</v>
       </c>
       <c r="I77" s="21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>50</v>
@@ -5158,15 +5161,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C78" s="30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>28</v>
@@ -5191,15 +5194,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>28</v>
@@ -5223,15 +5226,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>28</v>
@@ -5255,15 +5258,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C81" s="30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>28</v>
@@ -5272,16 +5275,16 @@
         <v>11</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I81" s="22" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>50</v>
@@ -5290,15 +5293,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>28</v>
@@ -5307,16 +5310,16 @@
         <v>11</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I82" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>50</v>
@@ -5325,15 +5328,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C83" s="30" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>28</v>
@@ -5342,16 +5345,16 @@
         <v>11</v>
       </c>
       <c r="F83" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H83" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I83" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>50</v>
@@ -5360,15 +5363,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C84" s="30" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>28</v>
@@ -5377,7 +5380,7 @@
         <v>11</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>19</v>
@@ -5386,7 +5389,7 @@
         <v>19</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>50</v>
@@ -5395,15 +5398,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C85" s="30" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>28</v>
@@ -5428,15 +5431,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C86" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>28</v>
@@ -5460,15 +5463,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C87" s="30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>28</v>
@@ -5477,7 +5480,7 @@
         <v>11</v>
       </c>
       <c r="F87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>19</v>
@@ -5486,7 +5489,7 @@
         <v>19</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>50</v>
@@ -5495,15 +5498,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C88" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>28</v>
@@ -5528,15 +5531,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C89" s="30" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>28</v>
@@ -5561,15 +5564,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>28</v>
@@ -5578,16 +5581,16 @@
         <v>11</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I90" s="23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>50</v>
@@ -5596,15 +5599,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C91" s="30" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>28</v>
@@ -5629,15 +5632,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C92" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>28</v>
@@ -5662,15 +5665,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C93" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>28</v>
@@ -5679,16 +5682,16 @@
         <v>11</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>50</v>
@@ -5697,15 +5700,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C94" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>28</v>
@@ -5714,7 +5717,7 @@
         <v>11</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>19</v>
@@ -5723,7 +5726,7 @@
         <v>19</v>
       </c>
       <c r="I94" s="21" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>50</v>
@@ -5732,15 +5735,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C95" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>28</v>
@@ -5749,16 +5752,16 @@
         <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H95" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>50</v>
@@ -5767,15 +5770,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>28</v>
@@ -5784,16 +5787,16 @@
         <v>11</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>50</v>
@@ -5802,15 +5805,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C97" s="30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>28</v>
@@ -5819,16 +5822,16 @@
         <v>11</v>
       </c>
       <c r="F97" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H97" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>50</v>
@@ -5837,15 +5840,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C98" s="30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>28</v>
@@ -5854,7 +5857,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>19</v>
@@ -5863,7 +5866,7 @@
         <v>19</v>
       </c>
       <c r="I98" s="21" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>50</v>
@@ -5872,15 +5875,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C99" s="30" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>28</v>
@@ -5904,15 +5907,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C100" s="30" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>28</v>
@@ -5937,15 +5940,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C101" s="30" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>28</v>
@@ -5954,7 +5957,7 @@
         <v>11</v>
       </c>
       <c r="F101" s="15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>19</v>
@@ -5963,7 +5966,7 @@
         <v>19</v>
       </c>
       <c r="I101" s="21" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>50</v>
@@ -5972,15 +5975,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C102" s="30" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>28</v>
@@ -5989,16 +5992,16 @@
         <v>11</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H102" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>50</v>
@@ -6007,15 +6010,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C103" s="30" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>28</v>
@@ -6024,16 +6027,16 @@
         <v>11</v>
       </c>
       <c r="F103" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H103" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>50</v>
@@ -6042,15 +6045,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>28</v>
@@ -6075,15 +6078,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>28</v>
@@ -6092,7 +6095,7 @@
         <v>11</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>19</v>
@@ -6101,7 +6104,7 @@
         <v>19</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>50</v>
@@ -6110,15 +6113,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C106" s="30" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>28</v>
@@ -6127,7 +6130,7 @@
         <v>11</v>
       </c>
       <c r="F106" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>19</v>
@@ -6136,7 +6139,7 @@
         <v>19</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>50</v>
@@ -6145,15 +6148,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C107" s="30" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>28</v>
@@ -6177,15 +6180,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C108" s="30" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>28</v>
@@ -6209,15 +6212,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C109" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>28</v>
@@ -6241,15 +6244,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C110" s="30" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>28</v>
@@ -6273,15 +6276,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C111" s="30" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>28</v>
@@ -6306,15 +6309,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C112" s="30" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>28</v>
@@ -6339,15 +6342,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C113" s="30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>28</v>
@@ -6372,15 +6375,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C114" s="30" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>28</v>
@@ -6405,15 +6408,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C115" s="30" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>28</v>
@@ -6438,15 +6441,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C116" s="30" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D116" s="7" t="s">
         <v>28</v>
@@ -6471,15 +6474,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C117" s="30" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>28</v>
@@ -6504,15 +6507,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C118" s="30" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>28</v>
@@ -6537,15 +6540,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C119" s="30" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D119" s="7" t="s">
         <v>28</v>
@@ -6569,15 +6572,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C120" s="30" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>28</v>
@@ -6601,15 +6604,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C121" s="30" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>28</v>
@@ -6633,15 +6636,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="6">
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C122" s="30" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>28</v>
@@ -6665,15 +6668,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="6">
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C123" s="30" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>28</v>
@@ -6697,15 +6700,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C124" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>28</v>
@@ -6729,15 +6732,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="6">
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C125" s="30" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>28</v>
@@ -6761,15 +6764,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C126" s="30" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>28</v>
@@ -6793,15 +6796,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="6">
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C127" s="30" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>28</v>
@@ -6825,15 +6828,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C128" s="30" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>28</v>
@@ -6857,15 +6860,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C129" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>17</v>
@@ -6874,16 +6877,16 @@
         <v>11</v>
       </c>
       <c r="F129" s="34" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H129">
         <v>5</v>
       </c>
       <c r="I129" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J129" s="35" t="s">
         <v>13</v>
@@ -6898,27 +6901,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -7159,32 +7141,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8FD927B-486E-4736-8E9F-ABBC39C726CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7201,4 +7179,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55D83430-B9A7-4A2C-B4EE-815D2E60FBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4056A9CA-2F02-448B-95FE-A9EC616FB2A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>